<commit_message>
Design integration test cases for v1
</commit_message>
<xml_diff>
--- a/Guru99/3 - Design & Execution/2 - Integration Testing/TestCases.xlsx
+++ b/Guru99/3 - Design & Execution/2 - Integration Testing/TestCases.xlsx
@@ -5,16 +5,16 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badri\Documents\GitHub\Manual-Testing\Guru99\3 - Design &amp; Execution\0 - Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badri\Documents\GitHub\Manual-Testing\Guru99\3 - Design &amp; Execution\2 - Integration Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7526A4A-661E-4301-9D52-1D035836F5AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB71479E-B4A5-4B43-8D3C-372C6BA1C3F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="3" r:id="rId1"/>
-    <sheet name="Module1" sheetId="5" r:id="rId2"/>
+    <sheet name="V1" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="85">
   <si>
     <t>ID</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Mohamed Elbadri</t>
   </si>
   <si>
-    <t>20/10/2023</t>
-  </si>
-  <si>
     <t>Data</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>Choose Module</t>
   </si>
   <si>
-    <t>New Customer</t>
-  </si>
-  <si>
     <t>Full Project</t>
   </si>
   <si>
@@ -129,14 +123,226 @@
     <t>Cycle 2</t>
   </si>
   <si>
-    <t>Verify  (Suite)</t>
+    <t>Verify manager functionality  (Suite)</t>
+  </si>
+  <si>
+    <t>TC_integration_001</t>
+  </si>
+  <si>
+    <t>Verify Manager can add new customer</t>
+  </si>
+  <si>
+    <t>Validate the manager can add new customer successfully with valid data</t>
+  </si>
+  <si>
+    <t>1 - website opened
+2 - manager already loged in 
+3 - new customer page is opened</t>
+  </si>
+  <si>
+    <t>message appears to the user that say the new customer is added successfully</t>
+  </si>
+  <si>
+    <t>TC_integration_002</t>
+  </si>
+  <si>
+    <t>TC_integration_003</t>
+  </si>
+  <si>
+    <t>TC_integration_004</t>
+  </si>
+  <si>
+    <t>TC_integration_005</t>
+  </si>
+  <si>
+    <t>TC_integration_006</t>
+  </si>
+  <si>
+    <t>TC_integration_007</t>
+  </si>
+  <si>
+    <t>TC_integration_008</t>
+  </si>
+  <si>
+    <t>TC_integration_009</t>
+  </si>
+  <si>
+    <t>TC_integration_010</t>
+  </si>
+  <si>
+    <t>TC_integration_011</t>
+  </si>
+  <si>
+    <t>TC_integration_012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate that the system refuse data 
+dublication when the manager try to create
+ new customer with valid data that
+ previously used in another customer </t>
+  </si>
+  <si>
+    <t>message appears to the user that say theis email is used before, try with another email</t>
+  </si>
+  <si>
+    <t>Verify Manager can edit customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate that the manager can
+edit customer info </t>
+  </si>
+  <si>
+    <t>1 - website opened
+2 - manager already loged in 
+3 - edit customer page is opened</t>
+  </si>
+  <si>
+    <t>message appears that say "customer info is updated successfully"</t>
+  </si>
+  <si>
+    <t>Validate that the customer new 
+info is updated successfully by 
+reedite the same customer again</t>
+  </si>
+  <si>
+    <t>the new data that previously edited should be updated successfully and appears in the right field</t>
+  </si>
+  <si>
+    <t>Validate that manager can 
+not edit customer info
+ with non existing customer ID (fake data)</t>
+  </si>
+  <si>
+    <t>userID - 123456
+first name - Samah
+last name - kofta
+birth day - 20/10/1988
+Address - saft allaban
+City - giza
+State - giza
+PIN - 666666
+Telephone - 016666666660
+Email - kofta@gmail.com</t>
+  </si>
+  <si>
+    <t>userID - 123456
+address - kafr tohormos</t>
+  </si>
+  <si>
+    <t>1 - enter the userID
+2 - click submit button
+3 - enter all required fields
+4 - click submit</t>
+  </si>
+  <si>
+    <t>userID - 654321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - enter the userID
+2 - click submit button
+</t>
+  </si>
+  <si>
+    <t>message appears to the user that say "the userID is wrong"</t>
+  </si>
+  <si>
+    <t>Validate that the manager can not modify 
+email info of the customers</t>
+  </si>
+  <si>
+    <t>email - mloha@gmail.com</t>
+  </si>
+  <si>
+    <t>message appears to the user that say "the data is not updated "</t>
+  </si>
+  <si>
+    <t>Verify Manager can delete customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate that the manager 
+can delete customer data </t>
+  </si>
+  <si>
+    <t>1 - website opened
+2 - manager already loged in 
+3 - delete customer page is opened</t>
+  </si>
+  <si>
+    <t>userID - 123456</t>
+  </si>
+  <si>
+    <t>message appears to the user that say "the CUSTOMER DATA IS SUCCESSFULLY deleted "</t>
+  </si>
+  <si>
+    <t>Validate that the customer data is successfully deleted by delete that same customer ID twice</t>
+  </si>
+  <si>
+    <t>message appears to the user that say "this customer id is not exist"</t>
+  </si>
+  <si>
+    <t>Validate that the customer data is successfully deleted by check if the manager can edit the info after delete it</t>
+  </si>
+  <si>
+    <t>Verify Manager can create new account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate that the manager can 
+create account for existing customer with valid data </t>
+  </si>
+  <si>
+    <t>1 - website opened
+2 - manager already loged in 
+3 - account page is opened</t>
+  </si>
+  <si>
+    <t>userID - 123456
+account type - saving
+deposite - 500</t>
+  </si>
+  <si>
+    <t>1 - enter UserID
+2 - choose the account type from the drop down list
+3 - enter the deposite value
+4 - click submit</t>
+  </si>
+  <si>
+    <t>message appears that say "account is created successfully"</t>
+  </si>
+  <si>
+    <t>Validate that the manager can 
+create multible accounts for the same customr</t>
+  </si>
+  <si>
+    <t>Validate that the account is created successfully by check for ministatment for the account ID</t>
+  </si>
+  <si>
+    <t>1 - website opened
+2 - manager already loged in 
+3 - account created
+4 - mini statements page is opened</t>
+  </si>
+  <si>
+    <t>accountID - 123</t>
+  </si>
+  <si>
+    <t>1 - enter the required fields
+2 - click submit</t>
+  </si>
+  <si>
+    <t>mini statements is generated successfully and the user can see it</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +408,12 @@
       <color theme="1"/>
       <name val="Agency FB"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -406,7 +618,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -428,6 +640,24 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -459,24 +689,6 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -489,13 +701,49 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Style 1" xfId="1" xr:uid="{48540A74-5A38-46CE-A885-A7DEB07E9381}"/>
     <cellStyle name="Style 2" xfId="2" xr:uid="{C54BD104-D706-4CC8-B1AF-F972C2684223}"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="33">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -613,86 +861,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -936,7 +1104,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{AB4FE4A9-2E76-4B1F-81EF-FEC07E8E0282}">
-      <tableStyleElement type="wholeTable" dxfId="37"/>
+      <tableStyleElement type="wholeTable" dxfId="32"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1218,7 +1386,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1526,7 +1694,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1926,16 +2094,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2035,7 +2203,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3990,15 +4158,15 @@
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{B72A5ACC-2E50-4F97-A328-3FEEF764509B}" name="#" dataDxfId="36" totalsRowDxfId="35" dataCellStyle="Style 2"/>
-    <tableColumn id="2" xr3:uid="{7CBB9464-FC05-4E8B-982E-2A12E8025BC6}" name="Data" dataDxfId="34" totalsRowDxfId="33" dataCellStyle="Style 2"/>
+    <tableColumn id="1" xr3:uid="{B72A5ACC-2E50-4F97-A328-3FEEF764509B}" name="#" dataDxfId="31" totalsRowDxfId="30" dataCellStyle="Style 2"/>
+    <tableColumn id="2" xr3:uid="{7CBB9464-FC05-4E8B-982E-2A12E8025BC6}" name="Data" dataDxfId="29" totalsRowDxfId="28" dataCellStyle="Style 2"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{0C31FF33-E6D9-449A-B3AF-85F8D5422CBE}" name="Table6" displayName="Table6" ref="N4:R6" headerRowDxfId="32" dataDxfId="31" totalsRowDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{0C31FF33-E6D9-449A-B3AF-85F8D5422CBE}" name="Table6" displayName="Table6" ref="N4:R6" headerRowDxfId="27" dataDxfId="26" totalsRowDxfId="25">
   <autoFilter ref="N4:R6" xr:uid="{0C31FF33-E6D9-449A-B3AF-85F8D5422CBE}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4007,13 +4175,13 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{9DBC923E-EFF7-49AB-A2ED-8B79F0C13714}" name="#" totalsRowLabel="Total" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{685A5DB2-DC97-4B8B-9E3F-436FCED90CA8}" name="Total TC" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{6B64B690-FCDB-4A7F-BD41-E98D9DFFD8BF}" name="Pass" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{56ECF0C6-8009-46E6-81D4-A0834F7D6873}" name="Fail" dataDxfId="24">
+    <tableColumn id="1" xr3:uid="{9DBC923E-EFF7-49AB-A2ED-8B79F0C13714}" name="#" totalsRowLabel="Total" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{685A5DB2-DC97-4B8B-9E3F-436FCED90CA8}" name="Total TC" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{6B64B690-FCDB-4A7F-BD41-E98D9DFFD8BF}" name="Pass" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{56ECF0C6-8009-46E6-81D4-A0834F7D6873}" name="Fail" dataDxfId="19">
       <calculatedColumnFormula>IF(G4="New Customer",COUNTIF(#REF!,"Fail"),IF(G4="Log",COUNTIF(#REF!,"Fail"),IF(G4="Edit Customer",COUNTIF(#REF!,"Fail"),0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{760B8D93-8EBC-4075-8646-91FA6A41FEBD}" name="Not Executed" totalsRowFunction="count" dataDxfId="23">
+    <tableColumn id="5" xr3:uid="{760B8D93-8EBC-4075-8646-91FA6A41FEBD}" name="Not Executed" totalsRowFunction="count" dataDxfId="18">
       <calculatedColumnFormula>IF(G3="New Customer",COUNTIF(#REF!,"Not Executed"),0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4288,7 +4456,7 @@
   <dimension ref="B1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4303,27 +4471,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="32.5" x14ac:dyDescent="0.65">
-      <c r="B1" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="10"/>
+      <c r="B1" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="16"/>
       <c r="H1" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
+        <v>20</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
     </row>
     <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:18" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -4333,25 +4501,25 @@
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="13"/>
+      <c r="G4" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" s="18"/>
+      <c r="I4" s="19"/>
       <c r="N4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="9" t="s">
-        <v>17</v>
-      </c>
       <c r="P4" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Q4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="R4" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="R4" s="9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:18" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -4361,92 +4529,92 @@
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="16"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="22"/>
       <c r="N5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="O5" s="9" t="e">
-        <f>IF(G4="New Customer",COUNTIF(#REF!,"*TC*"),IF(G4="Log",COUNTIF(#REF!,"*TC*"),IF(G4="Edit Customer",COUNTIF(#REF!,"*TC*"),0)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P5" s="9" t="e">
-        <f>IF(G4="New Customer",COUNTIF(#REF!,"PASS"),IF(G4="Log",COUNTIF(#REF!,"PASS"),IF(G4="Edit Customer",COUNTIF(#REF!,"PASS"),0)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q5" s="9" t="e">
-        <f>IF(G4="New Customer",COUNTIF(#REF!,"Fail"),IF(G4="Log",COUNTIF(#REF!,"Fail"),IF(G4="Edit Customer",COUNTIF(#REF!,"Fail"),0)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R5" s="9" t="e">
-        <f>IF(G4="New Customer",COUNTIF(#REF!,"Not Executed"),IF(G4="Log",COUNTIF(#REF!,"Not Executed"),IF(G4="Edit Customer",COUNTIF(#REF!,"Not Executed"),0)))</f>
-        <v>#REF!</v>
+        <v>23</v>
+      </c>
+      <c r="O5" s="9">
+        <f>IF(G4="v1",COUNTIF('V1'!A:H, "*integration*"),IF(G4="Log",COUNTIF(#REF!,"*TC*"),IF(G4="Edit Customer",COUNTIF(#REF!,"*TC*"),0)))</f>
+        <v>12</v>
+      </c>
+      <c r="P5" s="9">
+        <f>IF(G4="v1",COUNTIF('V1'!I:I,"PASS"),IF(G4="Log",COUNTIF(#REF!,"PASS"),IF(G4="Edit Customer",COUNTIF(#REF!,"PASS"),0)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q5" s="9">
+        <f>IF(G4="V1",COUNTIF('V1'!I:I,"Fail"),IF(G4="Log",COUNTIF(#REF!,"Fail"),IF(G4="Edit Customer",COUNTIF(#REF!,"Fail"),0)))</f>
+        <v>2</v>
+      </c>
+      <c r="R5" s="9">
+        <f>IF(G4="V1",COUNTIF('V1'!I:I,"Not Executed"),IF(G4="Log",COUNTIF(#REF!,"Not Executed"),IF(G4="Edit Customer",COUNTIF(#REF!,"Not Executed"),0)))</f>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:18" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="19"/>
+      <c r="C6" s="31">
+        <v>45383</v>
+      </c>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="25"/>
       <c r="N6" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="P6" s="9" t="e">
-        <f>IF(G4="New Customer",COUNTIF(#REF!,"PASS"),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q6" s="9" t="e">
-        <f>IF(G4="New Customer",COUNTIF(#REF!,"FAIL"),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R6" s="9" t="e">
-        <f>IF(G4="New Customer",COUNTIF(#REF!,"Not Executed"),0)</f>
-        <v>#REF!</v>
+        <v>15</v>
+      </c>
+      <c r="P6" s="9">
+        <f>IF(G4="V1",COUNTIF('V1'!L:L,"PASS"),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="9">
+        <f>IF(G4="v1",COUNTIF('V1'!L:L,"FAIL"),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R6" s="9">
+        <f>IF(G4="v1",COUNTIF('V1'!L:L,"Not Executed"),0)</f>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:18" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="1" t="e">
-        <f>SUM(COUNTIF(#REF!, "*TC*"),COUNTIF(#REF!, "*TC*"),COUNTIF(#REF!, "*TC*"),COUNTIF(Module1!A:A, "*TC*"),COUNTIF(#REF!, "*TC*"),COUNTIF(#REF!, "*TC*"))</f>
-        <v>#REF!</v>
+        <v>16</v>
+      </c>
+      <c r="C7" s="1">
+        <f>SUM(COUNTIF('V1'!A:H, "*integration*"))</f>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:18" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="1" t="e">
-        <f>SUM(COUNTIF(#REF!,"pass"),COUNTIF(#REF!,"pass"),COUNTIF(#REF!,"pass"),COUNTIF(Module1!A:J,"pass"))</f>
-        <v>#REF!</v>
+        <v>17</v>
+      </c>
+      <c r="C8" s="1">
+        <f>SUM(COUNTIF('V1'!A:H,"pass"))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:18" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="1" t="e">
-        <f>SUM(COUNTIF(#REF!,"fail"),COUNTIF(#REF!,"fail"),COUNTIF(#REF!,"fail"),COUNTIF(Module1!A:J,"fail"))</f>
-        <v>#REF!</v>
+        <v>18</v>
+      </c>
+      <c r="C9" s="1">
+        <f>SUM(COUNTIF('V1'!A:H,"fail"))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="1" t="e">
-        <f>SUM(COUNTIF(#REF!,"not executed"),COUNTIF(#REF!,"not executed"),COUNTIF(#REF!,"not executed"),COUNTIF(Module1!A:J,"not executed"),COUNTIF(#REF!, "not executed"),COUNTIF(#REF!, "not executed"))</f>
-        <v>#REF!</v>
+        <v>19</v>
+      </c>
+      <c r="C10" s="1">
+        <f>SUM(COUNTIF('V1'!A:H,"not executed"))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:18" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -4471,8 +4639,8 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" errorStyle="information" showInputMessage="1" showErrorMessage="1" sqref="G4" xr:uid="{714BD288-F0AA-464C-8AA8-06F6C0479280}">
-      <formula1>"Choose, Log, New Customer,Edit Customer"</formula1>
+    <dataValidation type="list" errorStyle="information" showInputMessage="1" showErrorMessage="1" sqref="G4:I6" xr:uid="{E987C23E-EB2F-40F0-BC42-0AF55EC81C9B}">
+      <formula1>"v1, v2, v3"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4508,19 +4676,21 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView zoomScale="31" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView zoomScale="27" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="45" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="14" width="50.6328125" style="4" customWidth="1"/>
+    <col min="1" max="2" width="50.6328125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="65.6328125" style="4" customWidth="1"/>
+    <col min="4" max="14" width="50.6328125" style="4" customWidth="1"/>
     <col min="15" max="16384" width="8.7265625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="55" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -4530,151 +4700,491 @@
       <c r="G1" s="27"/>
       <c r="H1" s="27"/>
       <c r="I1" s="28" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J1" s="28"/>
       <c r="K1" s="28"/>
       <c r="L1" s="29" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="M1" s="29"/>
       <c r="N1" s="29"/>
     </row>
     <row r="2" spans="1:14" ht="55" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="20" t="s">
+      <c r="J2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="20" t="s">
-        <v>27</v>
+      <c r="M2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="6" customFormat="1" ht="55" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22" t="s">
-        <v>20</v>
+    <row r="3" spans="1:14" s="6" customFormat="1" ht="261" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="11"/>
+      <c r="I3" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="J3" s="8"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
     </row>
-    <row r="4" spans="1:14" ht="55" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
+    <row r="4" spans="1:14" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="15"/>
+      <c r="I4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
     </row>
-    <row r="5" spans="1:14" ht="45" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5"/>
+    <row r="5" spans="1:14" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="15"/>
+      <c r="I5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
     </row>
-    <row r="6" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
+    <row r="6" spans="1:14" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="15"/>
+      <c r="I6" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
     </row>
-    <row r="7" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
+    <row r="7" spans="1:14" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="15"/>
+      <c r="I7" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
     </row>
-    <row r="8" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
+    <row r="8" spans="1:14" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="15"/>
+      <c r="I8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
     </row>
-    <row r="9" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
+    <row r="9" spans="1:14" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="15"/>
+      <c r="I9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
     </row>
-    <row r="10" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="5"/>
+    <row r="10" spans="1:14" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="15"/>
+      <c r="I10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
     </row>
-    <row r="11" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5"/>
+    <row r="11" spans="1:14" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
     </row>
-    <row r="12" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
+    <row r="12" spans="1:14" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" s="15"/>
+      <c r="I12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
     </row>
-    <row r="13" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="5"/>
+    <row r="13" spans="1:14" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
     </row>
-    <row r="14" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
+    <row r="14" spans="1:14" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="15"/>
+      <c r="I14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
     </row>
-    <row r="15" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="5"/>
+    <row r="15" spans="1:14" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
     </row>
-    <row r="16" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="5"/>
+    <row r="16" spans="1:14" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="8"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
     </row>
-    <row r="17" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="5"/>
+    <row r="17" spans="1:14" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="8"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
     </row>
-    <row r="18" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="5"/>
+    <row r="18" spans="1:14" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
     </row>
-    <row r="19" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" ht="45" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
     </row>
-    <row r="20" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
     </row>
-    <row r="21" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
     </row>
-    <row r="22" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
     </row>
-    <row r="23" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
     </row>
   </sheetData>
@@ -4683,74 +5193,75 @@
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="L1:N1"/>
   </mergeCells>
-  <conditionalFormatting sqref="I2:I3">
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+  <phoneticPr fontId="9" type="noConversion"/>
+  <conditionalFormatting sqref="I2:I17">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>"Not Executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+  <conditionalFormatting sqref="I3:I17">
+    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
       <formula>"Default"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="17" operator="equal">
       <formula>"fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="18" operator="equal">
       <formula>"pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:K2">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
       <formula>"Not Executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="12" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L3">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+  <conditionalFormatting sqref="L2:L17">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Not Executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+  <conditionalFormatting sqref="L3:L17">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Default"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>"pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:N2">
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>"Not Executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3 I3" xr:uid="{DF9BF969-6E47-47F0-AE8E-1764CDEDF07A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I14 L3:L14" xr:uid="{DF9BF969-6E47-47F0-AE8E-1764CDEDF07A}">
       <formula1>"Not Executed,PASS,FAIL"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>